<commit_message>
added uniqueness to hub_truckings and updated insertion query
Former-commit-id: 4ba36c7186d2836b3ca71e67016326ede8a3ad7b
</commit_message>
<xml_diff>
--- a/db/dummydata/new_gc_trucking_gothenburg_port_ftl.xlsx
+++ b/db/dummydata/new_gc_trucking_gothenburg_port_ftl.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">161-200</t>
   </si>
   <si>
-    <t xml:space="preserve">200-3000</t>
+    <t xml:space="preserve">201-3000</t>
   </si>
   <si>
     <t xml:space="preserve">FEE</t>
@@ -460,24 +460,24 @@
   <dimension ref="A1:AR1000"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="28" min="19" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="28" min="19" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -838,15 +838,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,10 +2179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2535,15 +2535,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,15 +3860,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5185,15 +5185,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6526,15 +6526,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7867,15 +7867,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9208,15 +9208,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10549,15 +10549,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>